<commit_message>
Feat: Add nova planilha de teste
</commit_message>
<xml_diff>
--- a/Rendimento.xlsx
+++ b/Rendimento.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28224"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACF553E7-05BB-42C3-B29A-C3022B449C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C34EECC-5DC1-462C-8392-C1113DECFE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Nome</t>
   </si>
@@ -43,12 +43,45 @@
   </si>
   <si>
     <t>Receita Gerada</t>
+  </si>
+  <si>
+    <t>Ana Oliveira</t>
+  </si>
+  <si>
+    <t>Bruno Lima</t>
+  </si>
+  <si>
+    <t>Carla Martins</t>
+  </si>
+  <si>
+    <t>Daniel Souza</t>
+  </si>
+  <si>
+    <t>Fernanda Silva</t>
+  </si>
+  <si>
+    <t>Gabriel Santos</t>
+  </si>
+  <si>
+    <t>Helena Rocha</t>
+  </si>
+  <si>
+    <t>Igor Ferreira</t>
+  </si>
+  <si>
+    <t>Julia Almeida</t>
+  </si>
+  <si>
+    <t>Lucas Correia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -60,27 +93,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor theme="6"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -88,70 +115,37 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="6" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="6" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="6" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="6" tint="0.39997558519241921"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="6" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="6" tint="0.39997558519241921"/>
-        </top>
-      </border>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -165,18 +159,66 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="0"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6"/>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="12" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -192,15 +234,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3115EEBA-9945-435A-A7ED-35175FEA4150}" name="Tabela1" displayName="Tabela1" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:D2" xr:uid="{3115EEBA-9945-435A-A7ED-35175FEA4150}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3DAA139-8369-4256-94B4-577E30BB5640}" name="Tabela1" displayName="Tabela1" ref="A1:D11" insertRowShift="1" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D11" xr:uid="{F3DAA139-8369-4256-94B4-577E30BB5640}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F105DBB5-C4FA-4FB4-AF0E-D8B9C28DED87}" name="Nome"/>
-    <tableColumn id="2" xr3:uid="{7F6D2A73-1174-47F0-8D3E-528A7176379B}" name="Horas Trabalhadas"/>
-    <tableColumn id="3" xr3:uid="{BB274DF3-3A44-4777-A315-1CB74EEC84E4}" name="Custo por Hora"/>
-    <tableColumn id="4" xr3:uid="{A0B15770-384F-4234-B5F6-349C58CE2829}" name="Receita Gerada"/>
+    <tableColumn id="1" xr3:uid="{2AA116E0-348A-418D-93A1-F71D1BE49493}" name="Nome" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{C6A23794-05CB-4112-B045-1EDC56EBDC8F}" name="Horas Trabalhadas" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{72C380F3-1E6B-4C35-8FC3-44B5746CE8D5}" name="Custo por Hora" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{D111222C-063D-4CA3-8D81-A3F9C3AAB2E3}" name="Receita Gerada" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleDark4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -521,22 +563,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -545,8 +587,148 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>160</v>
+      </c>
+      <c r="C2" s="1">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>140</v>
+      </c>
+      <c r="C3" s="1">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>155</v>
+      </c>
+      <c r="C4" s="1">
+        <v>38</v>
+      </c>
+      <c r="D4" s="1">
+        <v>11200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>170</v>
+      </c>
+      <c r="C5" s="1">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>150</v>
+      </c>
+      <c r="C6" s="1">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>165</v>
+      </c>
+      <c r="C7" s="1">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1">
+        <v>11900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>145</v>
+      </c>
+      <c r="C8" s="1">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>175</v>
+      </c>
+      <c r="C9" s="1">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>160</v>
+      </c>
+      <c r="C10" s="1">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>150</v>
+      </c>
+      <c r="C11" s="1">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>